<commit_message>
pip2 forces added - no bugs - 1250 frames
</commit_message>
<xml_diff>
--- a/results_G2/ch2_permation_residue_comb.xlsx
+++ b/results_G2/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,7 +518,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>130, 130, 426, 786</t>
+          <t>130, 426</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -578,20 +578,20 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>98, 130, 786, SF</t>
+          <t>130, 786</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>786</t>
+          <t>786, 130</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>959</t>
+          <t>959, 1219</t>
         </is>
       </c>
     </row>
@@ -618,7 +618,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>98, 130, 786, 1082</t>
+          <t>98, 786, 1082</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -638,7 +638,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>98, 426, 1082, SF, SF</t>
+          <t>98, 1082, SF</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -658,7 +658,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>98, 458, 754, 786, 1082</t>
+          <t>754, 786, 1082</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -678,7 +678,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>98, 458, 754, 1082</t>
+          <t>458</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -698,7 +698,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>130, 426, 786, SF, SF</t>
+          <t>786</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -712,26 +712,6 @@
       <c r="D14" t="inlineStr">
         <is>
           <t>1225</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>98, 130, 754, 786, 1082, SF</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>1219</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ionic up and ionic down forces added
</commit_message>
<xml_diff>
--- a/results_G2/ch2_permation_residue_comb.xlsx
+++ b/results_G2/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>98, 130, 786, 786</t>
+          <t>130, 130, 426, 786</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -466,19 +466,19 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>786</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>594</t>
+          <t>969</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>130, 426, 458</t>
+          <t>98, 458, 754, 1082</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>458</t>
+          <t>1082</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>692</t>
+          <t>946</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 130, 458</t>
+          <t>98, 130, 786, SF</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,212 +506,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>786</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>565</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>130, 426</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>969</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>130, 458, 754, 786</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>786</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>707</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>130, 786, 1082</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>787</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>130, 786</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>786, 130</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>959, 1219</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>130, 1082, 1114, SF</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1114</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>777</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>98, 786, 1082</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>786</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>794</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>98, 1082, SF</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>SF</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>806</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>754, 786, 1082</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1082</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>946</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>458</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>458</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>1186</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>786</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>786</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>1225</t>
+          <t>959</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed ions that do not permeate to appear with last frame as permeation frame
</commit_message>
<xml_diff>
--- a/results_G2/ch2_permation_residue_comb.xlsx
+++ b/results_G2/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,20 +458,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>130, 130, 426, 786</t>
+          <t>426, 754, 1082, SF</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>754, SF, 1082, 426</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>969</t>
+          <t>1248, 1248, 1248, 1248</t>
         </is>
       </c>
     </row>
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1082</t>
+          <t>458</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>946</t>
+          <t>1186</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>98, 130, 786, SF</t>
+          <t>130, 426, 786, SF, SF</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -511,7 +511,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>959</t>
+          <t>1225</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>98, 130, 754, 786, 1082, SF</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1219</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding coexisting ions folder and number of ions before permeation
</commit_message>
<xml_diff>
--- a/results_G2/ch2_permation_residue_comb.xlsx
+++ b/results_G2/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>98, 130, 786, 786</t>
+          <t>130, 786</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -471,14 +471,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>594</t>
+          <t>959</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>130, 426, 458</t>
+          <t>130</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>458</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>692</t>
+          <t>969</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>130, 130, 458</t>
+          <t>98, 1082, SF</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,19 +506,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>SF</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>565</t>
+          <t>806</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>130, 130, 426, 786</t>
+          <t>754, 786, 1082</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -526,232 +526,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>1082</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>969</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>130, 458, 754, 786</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>786</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>707</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>130, 786, 1082</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>787</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>98, 130, 786, SF</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>786</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>959</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>130, 1082, 1114, SF</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1114</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>777</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>426, 754, 1082, SF</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>4</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>754, SF, 1082, 426</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1248, 1248, 1248, 1248</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>98, 130, 786, 1082</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>786</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>794</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>98, 426, 1082, SF, SF</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>SF</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>806</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>98, 458, 754, 786, 1082</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1082</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
           <t>946</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>98, 458, 754, 1082</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>458</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>1186</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>130, 426, 786, SF, SF</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>786</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>1225</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>98, 130, 754, 786, 1082, SF</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>1219</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
before changes in SF as closest distance
</commit_message>
<xml_diff>
--- a/results_G2/ch2_permation_residue_comb.xlsx
+++ b/results_G2/ch2_permation_residue_comb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>130, 786</t>
+          <t>98, 130, 786, 786</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -471,14 +471,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>959</t>
+          <t>594</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>130, 426, 458</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,19 +486,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>458</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>969</t>
+          <t>692</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>98, 1082, SF</t>
+          <t>130, 130, 458</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,19 +506,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>130</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>806</t>
+          <t>565</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>754, 786, 1082</t>
+          <t>130, 130, 426, 786</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -526,12 +526,232 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>969</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>130, 458, 754, 786</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>786</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>707</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>130, 786, 1082</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>787</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>98, 130, 786, SF</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>786</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>959</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>130, 1082, 1114, SF</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1114</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>777</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>426, 754, 1082, SF</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>754, SF, 1082, 426</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1248, 1248, 1248, 1248</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>98, 130, 786, 1082</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>786</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>794</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>98, 426, 1082, SF, SF</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>806</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>98, 458, 754, 786, 1082</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>1082</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>946</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>98, 458, 754, 1082</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>458</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1186</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>130, 426, 786, SF, SF</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>786</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1225</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>98, 130, 754, 786, 1082, SF</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>1219</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changed SF condition, ion is in SF only if it has greater z than com of sf residues
</commit_message>
<xml_diff>
--- a/results_G2/ch2_permation_residue_comb.xlsx
+++ b/results_G2/ch2_permation_residue_comb.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -478,7 +478,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>130, 426, 458</t>
+          <t>130, 426, 458, SF</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -578,7 +578,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>98, 130, 786, SF</t>
+          <t>98, 130, 754, 786</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -598,7 +598,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>130, 1082, 1114, SF</t>
+          <t>130, 754, 1082, 1114</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -618,7 +618,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>426, 754, 1082, SF</t>
+          <t>426, 754, 1082, 1082</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -626,7 +626,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>754, SF, 1082, 426</t>
+          <t>754, 1082, 1082, 426</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -658,7 +658,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>98, 426, 1082, SF, SF</t>
+          <t>98, 130, 426, 426, 1082</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -666,7 +666,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>426</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -718,7 +718,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>130, 426, 786, SF, SF</t>
+          <t>98, 426, 426, 754, 786</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -738,7 +738,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>98, 130, 754, 786, 1082, SF</t>
+          <t>98, 130, 130, 426, 754, 1082</t>
         </is>
       </c>
       <c r="B16" t="n">

</xml_diff>